<commit_message>
commiting latest fixes to databases
</commit_message>
<xml_diff>
--- a/cea/databases/CH/archetypes/CONSTRUCTION_STANDARD.xlsx
+++ b/cea/databases/CH/archetypes/CONSTRUCTION_STANDARD.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2925" windowWidth="19335" windowHeight="16455" tabRatio="785" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2925" windowWidth="19335" windowHeight="16455" tabRatio="785" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="STANDARD_DEFINITION" sheetId="10" r:id="rId1"/>
@@ -165,51 +165,6 @@
     <t>STANDARD</t>
   </si>
   <si>
-    <t>WALL2</t>
-  </si>
-  <si>
-    <t>WALL5</t>
-  </si>
-  <si>
-    <t>SHADE2</t>
-  </si>
-  <si>
-    <t>SHADE1</t>
-  </si>
-  <si>
-    <t>ROOF2</t>
-  </si>
-  <si>
-    <t>ROOF1</t>
-  </si>
-  <si>
-    <t>ROOF4</t>
-  </si>
-  <si>
-    <t>WIN4</t>
-  </si>
-  <si>
-    <t>WIN2</t>
-  </si>
-  <si>
-    <t>WIN1</t>
-  </si>
-  <si>
-    <t>LEAK3</t>
-  </si>
-  <si>
-    <t>LEAK2</t>
-  </si>
-  <si>
-    <t>LEAK1</t>
-  </si>
-  <si>
-    <t>CONS3</t>
-  </si>
-  <si>
-    <t>CONS2</t>
-  </si>
-  <si>
     <t>STANDARD1</t>
   </si>
   <si>
@@ -310,6 +265,51 @@
   </si>
   <si>
     <t>HVAC_CONTROLLER_AS3</t>
+  </si>
+  <si>
+    <t>WALL_AS2</t>
+  </si>
+  <si>
+    <t>WALL_AS5</t>
+  </si>
+  <si>
+    <t>ROOF_AS2</t>
+  </si>
+  <si>
+    <t>ROOF_AS1</t>
+  </si>
+  <si>
+    <t>ROOF_AS4</t>
+  </si>
+  <si>
+    <t>SHADING_AS2</t>
+  </si>
+  <si>
+    <t>SHADING_AS1</t>
+  </si>
+  <si>
+    <t>WINDOW_AS1</t>
+  </si>
+  <si>
+    <t>WINDOW_AS2</t>
+  </si>
+  <si>
+    <t>WINDOW_AS4</t>
+  </si>
+  <si>
+    <t>TIGHTNESS_AS3</t>
+  </si>
+  <si>
+    <t>TIGHTNESS_AS2</t>
+  </si>
+  <si>
+    <t>TIGHTNESS_AS1</t>
+  </si>
+  <si>
+    <t>CONSTRUCTION_AS3</t>
+  </si>
+  <si>
+    <t>CONSTRUCTION_AS2</t>
   </si>
 </sst>
 </file>
@@ -1236,21 +1236,21 @@
         <v>42</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="D2" s="19">
         <v>1920</v>
@@ -1258,13 +1258,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="18" t="s">
         <v>60</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>75</v>
       </c>
       <c r="D3" s="19">
         <v>1970</v>
@@ -1272,13 +1272,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>61</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>76</v>
       </c>
       <c r="D4" s="19">
         <v>1980</v>
@@ -1286,13 +1286,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>62</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>77</v>
       </c>
       <c r="D5" s="19">
         <v>2000</v>
@@ -1300,13 +1300,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="D6" s="20">
         <v>2020</v>
@@ -1314,13 +1314,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="D7" s="20">
         <v>2020</v>
@@ -1338,21 +1338,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1:B1048576"/>
+      <selection pane="bottomRight" activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.140625" style="3" bestFit="1" customWidth="1"/>
@@ -1417,25 +1418,25 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="H2" s="2">
         <v>0.82</v>
@@ -1468,25 +1469,25 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="H3" s="2">
         <v>0.82</v>
@@ -1519,25 +1520,25 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="H4" s="2">
         <v>0.82</v>
@@ -1570,25 +1571,25 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="H5" s="2">
         <v>0.82</v>
@@ -1621,25 +1622,25 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="H6" s="2">
         <v>0.82</v>
@@ -1671,25 +1672,25 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>56</v>
+        <v>90</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="H7" s="2">
         <v>0.82</v>
@@ -1783,22 +1784,22 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>19</v>
@@ -1815,22 +1816,22 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>19</v>
@@ -1847,22 +1848,22 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>19</v>
@@ -1879,22 +1880,22 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>19</v>
@@ -1911,22 +1912,22 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>19</v>
@@ -1943,22 +1944,22 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>19</v>
@@ -1983,7 +1984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
@@ -2016,104 +2017,104 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -2190,7 +2191,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B2" s="9">
         <v>57</v>
@@ -2231,7 +2232,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B3" s="9">
         <v>34</v>
@@ -2272,7 +2273,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="B4" s="9">
         <v>36</v>
@@ -2313,7 +2314,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B5" s="9">
         <v>57</v>
@@ -2354,7 +2355,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B6" s="9">
         <v>112</v>
@@ -2395,7 +2396,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="B7" s="9">
         <v>112</v>
@@ -2447,6 +2448,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C4119BA2A2C9A34A9ABDCD539C093B2A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2036187cb88b360b5a6de576d0a5f2f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="be70d004-d1e5-4317-a402-eff109a4a2bb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e63961df46f11abd186e13992df6f3c7" ns3:_="">
     <xsd:import namespace="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
@@ -2616,15 +2626,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
   <ds:schemaRefs>
@@ -2642,6 +2643,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02AC8DD-FE6B-486F-A4E4-4D415B112715}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2657,12 +2666,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
taking aout emissions intensity
</commit_message>
<xml_diff>
--- a/cea/databases/CH/archetypes/CONSTRUCTION_STANDARD.xlsx
+++ b/cea/databases/CH/archetypes/CONSTRUCTION_STANDARD.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="86">
   <si>
     <t>type_hs</t>
   </si>
@@ -282,6 +282,12 @@
   </si>
   <si>
     <t>FLOOR_AS2</t>
+  </si>
+  <si>
+    <t>type_part</t>
+  </si>
+  <si>
+    <t>WALL_AS7</t>
   </si>
 </sst>
 </file>
@@ -1291,13 +1297,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,22 +1313,22 @@
     <col min="3" max="3" width="15" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" style="1" customWidth="1"/>
-    <col min="7" max="8" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="7" width="11" style="1" customWidth="1"/>
+    <col min="8" max="9" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
@@ -1339,46 +1345,49 @@
         <v>7</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -1395,19 +1404,19 @@
         <v>67</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="H2" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="I2" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="J2" s="2">
-        <v>0.82</v>
       </c>
       <c r="K2" s="2">
         <v>0.82</v>
@@ -1415,14 +1424,14 @@
       <c r="L2" s="2">
         <v>0.82</v>
       </c>
-      <c r="M2" s="8">
+      <c r="M2" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="N2" s="8">
         <v>0</v>
       </c>
-      <c r="N2" s="7">
+      <c r="O2" s="7">
         <v>0</v>
-      </c>
-      <c r="O2" s="2">
-        <v>0.16</v>
       </c>
       <c r="P2" s="2">
         <v>0.16</v>
@@ -1433,9 +1442,12 @@
       <c r="R2" s="2">
         <v>0.16</v>
       </c>
-      <c r="S2" s="6"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S2" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="T2" s="6"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
@@ -1452,19 +1464,19 @@
         <v>67</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="H3" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="I3" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="J3" s="2">
-        <v>0.82</v>
       </c>
       <c r="K3" s="2">
         <v>0.82</v>
@@ -1472,14 +1484,14 @@
       <c r="L3" s="2">
         <v>0.82</v>
       </c>
-      <c r="M3" s="8">
+      <c r="M3" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="N3" s="8">
         <v>0</v>
       </c>
-      <c r="N3" s="7">
+      <c r="O3" s="7">
         <v>0</v>
-      </c>
-      <c r="O3" s="2">
-        <v>0.21</v>
       </c>
       <c r="P3" s="2">
         <v>0.21</v>
@@ -1490,9 +1502,12 @@
       <c r="R3" s="2">
         <v>0.21</v>
       </c>
-      <c r="S3" s="6"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S3" s="2">
+        <v>0.21</v>
+      </c>
+      <c r="T3" s="6"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
@@ -1509,19 +1524,19 @@
         <v>67</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="H4" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="I4" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0.82</v>
       </c>
       <c r="K4" s="2">
         <v>0.82</v>
@@ -1529,14 +1544,14 @@
       <c r="L4" s="2">
         <v>0.82</v>
       </c>
-      <c r="M4" s="8">
+      <c r="M4" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="N4" s="8">
         <v>0</v>
       </c>
-      <c r="N4" s="7">
+      <c r="O4" s="7">
         <v>0</v>
-      </c>
-      <c r="O4" s="2">
-        <v>0.25</v>
       </c>
       <c r="P4" s="2">
         <v>0.25</v>
@@ -1547,9 +1562,12 @@
       <c r="R4" s="2">
         <v>0.25</v>
       </c>
-      <c r="S4" s="6"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S4" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="T4" s="6"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -1566,19 +1584,19 @@
         <v>68</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="H5" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="I5" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0.82</v>
       </c>
       <c r="K5" s="2">
         <v>0.82</v>
@@ -1586,14 +1604,14 @@
       <c r="L5" s="2">
         <v>0.82</v>
       </c>
-      <c r="M5" s="8">
+      <c r="M5" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="N5" s="8">
         <v>0</v>
       </c>
-      <c r="N5" s="7">
+      <c r="O5" s="7">
         <v>0</v>
-      </c>
-      <c r="O5" s="2">
-        <v>0.21</v>
       </c>
       <c r="P5" s="2">
         <v>0.21</v>
@@ -1604,9 +1622,12 @@
       <c r="R5" s="2">
         <v>0.21</v>
       </c>
-      <c r="S5" s="6"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S5" s="2">
+        <v>0.21</v>
+      </c>
+      <c r="T5" s="6"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -1623,19 +1644,19 @@
         <v>69</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="H6" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="I6" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0.82</v>
       </c>
       <c r="K6" s="2">
         <v>0.82</v>
@@ -1643,14 +1664,14 @@
       <c r="L6" s="2">
         <v>0.82</v>
       </c>
-      <c r="M6" s="8">
+      <c r="M6" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="N6" s="8">
         <v>0</v>
       </c>
-      <c r="N6" s="7">
+      <c r="O6" s="7">
         <v>0</v>
-      </c>
-      <c r="O6" s="2">
-        <v>0.15</v>
       </c>
       <c r="P6" s="2">
         <v>0.15</v>
@@ -1661,8 +1682,11 @@
       <c r="R6" s="2">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S6" s="2">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
@@ -1679,19 +1703,19 @@
         <v>69</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="H7" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="I7" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="J7" s="2">
-        <v>0.82</v>
       </c>
       <c r="K7" s="2">
         <v>0.82</v>
@@ -1699,14 +1723,14 @@
       <c r="L7" s="2">
         <v>0.82</v>
       </c>
-      <c r="M7" s="8">
+      <c r="M7" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="N7" s="8">
         <v>0</v>
       </c>
-      <c r="N7" s="7">
+      <c r="O7" s="7">
         <v>0</v>
-      </c>
-      <c r="O7" s="2">
-        <v>0.15</v>
       </c>
       <c r="P7" s="2">
         <v>0.15</v>
@@ -1715,6 +1739,9 @@
         <v>0.15</v>
       </c>
       <c r="R7" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="S7" s="2">
         <v>0.15</v>
       </c>
     </row>
@@ -2121,6 +2148,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C4119BA2A2C9A34A9ABDCD539C093B2A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2036187cb88b360b5a6de576d0a5f2f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="be70d004-d1e5-4317-a402-eff109a4a2bb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e63961df46f11abd186e13992df6f3c7" ns3:_="">
     <xsd:import namespace="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
@@ -2290,35 +2332,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02AC8DD-FE6B-486F-A4E4-4D415B112715}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2340,9 +2357,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02AC8DD-FE6B-486F-A4E4-4D415B112715}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update year end to 2040
</commit_message>
<xml_diff>
--- a/cea/databases/CH/archetypes/CONSTRUCTION_STANDARD.xlsx
+++ b/cea/databases/CH/archetypes/CONSTRUCTION_STANDARD.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JimenoF\Documents\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\CH\archetypes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\CH\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2925" windowWidth="19335" windowHeight="16455" tabRatio="785" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2930" windowWidth="19340" windowHeight="16460" tabRatio="785"/>
   </bookViews>
   <sheets>
     <sheet name="STANDARD_DEFINITION" sheetId="10" r:id="rId1"/>
@@ -1177,19 +1177,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>1970</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -1270,10 +1270,10 @@
         <v>46</v>
       </c>
       <c r="D6" s="12">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>46</v>
       </c>
       <c r="D7" s="12">
-        <v>2020</v>
+        <v>2040</v>
       </c>
     </row>
   </sheetData>
@@ -1299,36 +1299,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.54296875" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="11" style="1" customWidth="1"/>
-    <col min="8" max="9" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.26953125" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="1"/>
+    <col min="16" max="16" width="10.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="T2" s="6"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
@@ -1507,7 +1507,7 @@
       </c>
       <c r="T3" s="6"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
@@ -1567,7 +1567,7 @@
       </c>
       <c r="T4" s="6"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -1627,7 +1627,7 @@
       </c>
       <c r="T5" s="6"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
@@ -1762,20 +1762,20 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="11.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.54296875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="21.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
@@ -2013,17 +2013,17 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="11.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
@@ -2148,21 +2148,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C4119BA2A2C9A34A9ABDCD539C093B2A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2036187cb88b360b5a6de576d0a5f2f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="be70d004-d1e5-4317-a402-eff109a4a2bb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e63961df46f11abd186e13992df6f3c7" ns3:_="">
     <xsd:import namespace="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
@@ -2332,10 +2317,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02AC8DD-FE6B-486F-A4E4-4D415B112715}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2357,19 +2367,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02AC8DD-FE6B-486F-A4E4-4D415B112715}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add missing floor assemblies and update construction standards
</commit_message>
<xml_diff>
--- a/cea/databases/CH/archetypes/CONSTRUCTION_STANDARD.xlsx
+++ b/cea/databases/CH/archetypes/CONSTRUCTION_STANDARD.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\CH\archetypes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Assistenz\Documents\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\CH\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2930" windowWidth="19340" windowHeight="16460" tabRatio="785"/>
+    <workbookView xWindow="0" yWindow="2925" windowWidth="19335" windowHeight="16455" tabRatio="785" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="STANDARD_DEFINITION" sheetId="10" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="87">
   <si>
     <t>type_hs</t>
   </si>
@@ -281,13 +281,16 @@
     <t>type_base</t>
   </si>
   <si>
-    <t>FLOOR_AS2</t>
-  </si>
-  <si>
     <t>type_part</t>
   </si>
   <si>
     <t>WALL_AS7</t>
+  </si>
+  <si>
+    <t>FLOOR_AS4</t>
+  </si>
+  <si>
+    <t>FLOOR_AS3</t>
   </si>
 </sst>
 </file>
@@ -1177,19 +1180,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
@@ -1203,7 +1206,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -1217,7 +1220,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
@@ -1231,7 +1234,7 @@
         <v>1970</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
@@ -1245,7 +1248,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -1259,7 +1262,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -1273,7 +1276,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
@@ -1299,36 +1302,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="11" style="1" customWidth="1"/>
-    <col min="8" max="9" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.1796875" style="1"/>
+    <col min="16" max="16" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
@@ -1345,7 +1348,7 @@
         <v>7</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>6</v>
@@ -1387,7 +1390,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -1404,7 +1407,7 @@
         <v>67</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>65</v>
@@ -1413,7 +1416,7 @@
         <v>80</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>70</v>
@@ -1447,7 +1450,7 @@
       </c>
       <c r="T2" s="6"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
@@ -1464,16 +1467,16 @@
         <v>67</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>66</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>71</v>
@@ -1507,7 +1510,7 @@
       </c>
       <c r="T3" s="6"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
@@ -1524,16 +1527,16 @@
         <v>67</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>66</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>71</v>
@@ -1567,7 +1570,7 @@
       </c>
       <c r="T4" s="6"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -1584,16 +1587,16 @@
         <v>68</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>66</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>71</v>
@@ -1627,7 +1630,7 @@
       </c>
       <c r="T5" s="6"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -1644,16 +1647,16 @@
         <v>69</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>66</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>71</v>
@@ -1686,7 +1689,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
@@ -1703,16 +1706,16 @@
         <v>69</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>66</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>71</v>
@@ -1762,20 +1765,20 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.54296875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="21.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
@@ -1807,7 +1810,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -1839,7 +1842,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
@@ -1871,7 +1874,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
@@ -1903,7 +1906,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -1935,7 +1938,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -1967,7 +1970,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
@@ -2013,17 +2016,17 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
@@ -2040,7 +2043,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -2057,7 +2060,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
@@ -2074,7 +2077,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
@@ -2091,7 +2094,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -2108,7 +2111,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -2125,7 +2128,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
@@ -2148,6 +2151,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C4119BA2A2C9A34A9ABDCD539C093B2A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2036187cb88b360b5a6de576d0a5f2f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="be70d004-d1e5-4317-a402-eff109a4a2bb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e63961df46f11abd186e13992df6f3c7" ns3:_="">
     <xsd:import namespace="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
@@ -2317,35 +2335,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02AC8DD-FE6B-486F-A4E4-4D415B112715}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2367,9 +2360,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02AC8DD-FE6B-486F-A4E4-4D415B112715}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update basement as well
</commit_message>
<xml_diff>
--- a/cea/databases/CH/archetypes/CONSTRUCTION_STANDARD.xlsx
+++ b/cea/databases/CH/archetypes/CONSTRUCTION_STANDARD.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Assistenz\Documents\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\CH\archetypes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Assistenz\Desktop\REMoD\Case_studies\Bonstetten_Wettswil\inputs\technology\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="88">
   <si>
     <t>type_hs</t>
   </si>
@@ -291,6 +291,9 @@
   </si>
   <si>
     <t>FLOOR_AS3</t>
+  </si>
+  <si>
+    <t>FLOOR_AS6</t>
   </si>
 </sst>
 </file>
@@ -1306,7 +1309,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomRight" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1476,7 +1479,7 @@
         <v>86</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>71</v>
@@ -1536,7 +1539,7 @@
         <v>86</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>71</v>
@@ -1596,7 +1599,7 @@
         <v>86</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>71</v>
@@ -1656,7 +1659,7 @@
         <v>86</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>71</v>
@@ -1715,7 +1718,7 @@
         <v>86</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>71</v>
@@ -2151,21 +2154,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C4119BA2A2C9A34A9ABDCD539C093B2A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2036187cb88b360b5a6de576d0a5f2f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="be70d004-d1e5-4317-a402-eff109a4a2bb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e63961df46f11abd186e13992df6f3c7" ns3:_="">
     <xsd:import namespace="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
@@ -2335,31 +2323,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02AC8DD-FE6B-486F-A4E4-4D415B112715}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2375,4 +2354,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
chancges to all databases of archetypes
</commit_message>
<xml_diff>
--- a/cea/databases/CH/archetypes/CONSTRUCTION_STANDARD.xlsx
+++ b/cea/databases/CH/archetypes/CONSTRUCTION_STANDARD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ebpgroup-my.sharepoint.com/personal/jimeno_fonseca_ebp_ch/Documents/Dokumente/CityEnergyAnalyst/CityEnergyAnalyst/cea/databases/CH/archetypes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="11_FC738FCD21D91416D512F37F2E5BB974BC1D8DF6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8238AD29-3865-4037-A7D8-D42FC724C48C}"/>
+  <xr:revisionPtr revIDLastSave="471" documentId="11_FC738FCD21D91416D512F37F2E5BB974BC1D8DF6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FB0E5ED-AA3B-4C0D-BC20-0DCE6CF98640}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="105" windowWidth="38640" windowHeight="21240" tabRatio="785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="785" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STANDARD_DEFINITION" sheetId="10" r:id="rId1"/>
@@ -18,10 +18,19 @@
     <sheet name="HVAC_ASSEMBLIES" sheetId="1" r:id="rId3"/>
     <sheet name="SUPPLY_ASSEMBLIES" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="146">
   <si>
     <t>type_hs</t>
   </si>
@@ -144,24 +153,9 @@
     <t>STANDARD6</t>
   </si>
   <si>
-    <t>Stone and Masonry from 1000's to 1920's</t>
-  </si>
-  <si>
-    <t>Concrete and Masonry from 1920's to 1970's</t>
-  </si>
-  <si>
     <t>Concrete and Masonry from 1970's to 1980's</t>
   </si>
   <si>
-    <t>Concrete and Masonry from 1980's to 2000's</t>
-  </si>
-  <si>
-    <t>Concrete and Masonry from 2000's to 2020's</t>
-  </si>
-  <si>
-    <t>Concrete and Masonry  from 2000's to 2020's - Minergie Standard</t>
-  </si>
-  <si>
     <t>YEAR_START</t>
   </si>
   <si>
@@ -171,12 +165,6 @@
     <t>1000</t>
   </si>
   <si>
-    <t>2000</t>
-  </si>
-  <si>
-    <t>1921</t>
-  </si>
-  <si>
     <t>1971</t>
   </si>
   <si>
@@ -285,21 +273,9 @@
     <t>type_part</t>
   </si>
   <si>
-    <t>WALL_AS7</t>
-  </si>
-  <si>
-    <t>FLOOR_AS4</t>
-  </si>
-  <si>
     <t>FLOOR_AS3</t>
   </si>
   <si>
-    <t>FLOOR_AS6</t>
-  </si>
-  <si>
-    <t>WALL_AS9</t>
-  </si>
-  <si>
     <t>WALL_AS10</t>
   </si>
   <si>
@@ -310,6 +286,198 @@
   </si>
   <si>
     <t>area_pv</t>
+  </si>
+  <si>
+    <t>SATANDARD1</t>
+  </si>
+  <si>
+    <t>SATANDARD2</t>
+  </si>
+  <si>
+    <t>SATANDARD3</t>
+  </si>
+  <si>
+    <t>SATANDARD4</t>
+  </si>
+  <si>
+    <t>SATANDARD5</t>
+  </si>
+  <si>
+    <t>SATANDARD6</t>
+  </si>
+  <si>
+    <t>SATANDARD7</t>
+  </si>
+  <si>
+    <t>SATANDARD8</t>
+  </si>
+  <si>
+    <t>SATANDARD9</t>
+  </si>
+  <si>
+    <t>SATANDARD10</t>
+  </si>
+  <si>
+    <t>SATANDARD11</t>
+  </si>
+  <si>
+    <t>SATANDARD12</t>
+  </si>
+  <si>
+    <t>STANDARD7</t>
+  </si>
+  <si>
+    <t>STANDARD8</t>
+  </si>
+  <si>
+    <t>STANDARD9</t>
+  </si>
+  <si>
+    <t>STANDARD10</t>
+  </si>
+  <si>
+    <t>TIGHTNESS_AS4</t>
+  </si>
+  <si>
+    <t>TIGHTNESS_AS5</t>
+  </si>
+  <si>
+    <t>TIGHTNESS_AS6</t>
+  </si>
+  <si>
+    <t>WINDOW_AS3</t>
+  </si>
+  <si>
+    <t>Stone and Masonry before 1900's</t>
+  </si>
+  <si>
+    <t>1901</t>
+  </si>
+  <si>
+    <t>Concrete and Masonry from 1900's to 1930's</t>
+  </si>
+  <si>
+    <t>1931</t>
+  </si>
+  <si>
+    <t>Concrete and Masonry from 1930s to 1960's</t>
+  </si>
+  <si>
+    <t>Concrete and Masonry from 1960's to 1970's</t>
+  </si>
+  <si>
+    <t>Concrete and Masonry from 1980's to 1990's</t>
+  </si>
+  <si>
+    <t>Concrete and Masonry (Minergie A)</t>
+  </si>
+  <si>
+    <t>1961</t>
+  </si>
+  <si>
+    <t>1990</t>
+  </si>
+  <si>
+    <t>SATANDARD13</t>
+  </si>
+  <si>
+    <t>SATANDARD14</t>
+  </si>
+  <si>
+    <t>SATANDARD15</t>
+  </si>
+  <si>
+    <t>Concrete and Masonry from 1990's to 2000's</t>
+  </si>
+  <si>
+    <t>1991</t>
+  </si>
+  <si>
+    <t>Concrete and Masonry from 2000's to 2010's</t>
+  </si>
+  <si>
+    <t>Concrete and Masonry from 2010's to 2020's</t>
+  </si>
+  <si>
+    <t>2001</t>
+  </si>
+  <si>
+    <t>2011</t>
+  </si>
+  <si>
+    <t>SATANDARD16</t>
+  </si>
+  <si>
+    <t>SATANDARD17</t>
+  </si>
+  <si>
+    <t>ROOF_AS3</t>
+  </si>
+  <si>
+    <t>Stone and Masonry before 1900's (renovated)</t>
+  </si>
+  <si>
+    <t>Concrete and Masonry from 1900's to 1930's  (renovated)</t>
+  </si>
+  <si>
+    <t>Concrete and Masonry from 1930s to 1960's  (renovated)</t>
+  </si>
+  <si>
+    <t>Concrete and Masonry from 1960's to 1970's  (renovated)</t>
+  </si>
+  <si>
+    <t>Concrete and Masonry from 1970's to 1980's  (renovated)</t>
+  </si>
+  <si>
+    <t>Concrete and Masonry from 1980's to 1990's  (renovated)</t>
+  </si>
+  <si>
+    <t>Concrete and Masonry from 1990's to 2000's  (renovated)</t>
+  </si>
+  <si>
+    <t>Refernez</t>
+  </si>
+  <si>
+    <t>1.3 Gebäudehülle seit 1900 | Bautechnik der Gebäudehülle (enbau-online.ch)</t>
+  </si>
+  <si>
+    <t>WALL_AS1</t>
+  </si>
+  <si>
+    <t>WALL_AS3</t>
+  </si>
+  <si>
+    <t>WALL_AS4</t>
+  </si>
+  <si>
+    <t>WALL_AS8</t>
+  </si>
+  <si>
+    <t>WALL_AS11</t>
+  </si>
+  <si>
+    <t>FLOOR_AS2</t>
+  </si>
+  <si>
+    <t>STANDARD11</t>
+  </si>
+  <si>
+    <t>STANDARD12</t>
+  </si>
+  <si>
+    <t>STANDARD13</t>
+  </si>
+  <si>
+    <t>STANDARD14</t>
+  </si>
+  <si>
+    <t>STANDARD15</t>
+  </si>
+  <si>
+    <t>STANDARD16</t>
+  </si>
+  <si>
+    <t>STANDARD17</t>
   </si>
 </sst>
 </file>
@@ -319,7 +487,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -453,6 +621,30 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="35">
@@ -779,7 +971,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -822,8 +1014,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -859,8 +1052,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -891,6 +1093,7 @@
     <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Link" xfId="42" builtinId="8"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
@@ -1180,15 +1383,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
     <col min="2" max="2" width="59.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
@@ -1202,871 +1405,2348 @@
         <v>29</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>37</v>
+        <v>102</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D2" s="10">
-        <v>1920</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>47</v>
+        <v>103</v>
       </c>
       <c r="D3" s="10">
-        <v>1970</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>39</v>
+        <v>106</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>48</v>
+        <v>105</v>
       </c>
       <c r="D4" s="10">
-        <v>1980</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>40</v>
+        <v>107</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>49</v>
+        <v>110</v>
       </c>
       <c r="D5" s="10">
-        <v>2000</v>
+        <v>1970</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>35</v>
+        <v>86</v>
       </c>
       <c r="B6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="11">
-        <v>2040</v>
+      <c r="D6" s="10">
+        <v>1980</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>36</v>
+        <v>87</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>46</v>
-      </c>
       <c r="D7" s="11">
-        <v>2040</v>
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D8" s="11">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D9" s="11">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" s="11">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" s="11">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="10">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" s="10">
+        <v>1930</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" s="10">
+        <v>1960</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D15" s="10">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="10">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="11">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D18" s="11">
+        <v>2000</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="C2:D3 C4:C7" numberStoredAsText="1"/>
+    <ignoredError sqref="C11 C2:C8 C9:C10 C12:D18" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:V7"/>
+  <dimension ref="A1:Y18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U2" sqref="U2"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="50" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="11" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X1" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="Y1" s="15"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="13" t="str">
+        <f>STANDARD_DEFINITION!B2</f>
+        <v>Stone and Masonry before 1900's</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M2" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="N2" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="O2" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="P2" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>0</v>
+      </c>
+      <c r="R2" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="S2" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="T2" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="U2" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="V2" s="6">
+        <v>0</v>
+      </c>
+      <c r="W2" s="6">
+        <v>0</v>
+      </c>
+      <c r="X2" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y2" s="15"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="B3" s="13" t="str">
+        <f>STANDARD_DEFINITION!B3</f>
+        <v>Concrete and Masonry from 1900's to 1930's</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="N3" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="O3" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="P3" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>0</v>
+      </c>
+      <c r="R3" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="S3" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="T3" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="U3" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="V3" s="6">
+        <v>0</v>
+      </c>
+      <c r="W3" s="6">
+        <v>0</v>
+      </c>
+      <c r="X3" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y3" s="15"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="13" t="str">
+        <f>STANDARD_DEFINITION!B4</f>
+        <v>Concrete and Masonry from 1930s to 1960's</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="P4" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="S4" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="T4" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="U4" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="V4" s="6">
+        <v>0</v>
+      </c>
+      <c r="W4" s="6">
+        <v>0</v>
+      </c>
+      <c r="X4" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y4" s="15"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="13" t="str">
+        <f>STANDARD_DEFINITION!B5</f>
+        <v>Concrete and Masonry from 1960's to 1970's</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="O5" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="P5" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>0</v>
+      </c>
+      <c r="R5" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="S5" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="T5" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="U5" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="V5" s="6">
+        <v>0</v>
+      </c>
+      <c r="W5" s="6">
+        <v>0</v>
+      </c>
+      <c r="X5" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y5" s="15"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="13" t="str">
+        <f>STANDARD_DEFINITION!B6</f>
+        <v>Concrete and Masonry from 1970's to 1980's</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="P6" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>0</v>
+      </c>
+      <c r="R6" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="S6" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="T6" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="U6" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="V6" s="6">
+        <v>0</v>
+      </c>
+      <c r="W6" s="6">
+        <v>0</v>
+      </c>
+      <c r="X6" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y6" s="15"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="13" t="str">
+        <f>STANDARD_DEFINITION!B7</f>
+        <v>Concrete and Masonry from 1980's to 1990's</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="P7" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="6">
+        <v>0</v>
+      </c>
+      <c r="R7" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="S7" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="T7" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="U7" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="V7" s="6">
+        <v>0</v>
+      </c>
+      <c r="W7" s="6">
+        <v>0</v>
+      </c>
+      <c r="X7" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y7" s="15"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="13" t="str">
+        <f>STANDARD_DEFINITION!B8</f>
+        <v>Concrete and Masonry from 1990's to 2000's</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="N8" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="O8" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="P8" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>0</v>
+      </c>
+      <c r="R8" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="S8" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="T8" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="U8" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="V8" s="6">
+        <v>0</v>
+      </c>
+      <c r="W8" s="6">
+        <v>0</v>
+      </c>
+      <c r="X8" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y8" s="15"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="13" t="str">
+        <f>STANDARD_DEFINITION!B9</f>
+        <v>Concrete and Masonry from 2000's to 2010's</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="O9" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="P9" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>0</v>
+      </c>
+      <c r="R9" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="S9" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="T9" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="U9" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="V9" s="6">
+        <v>0</v>
+      </c>
+      <c r="W9" s="6">
+        <v>0</v>
+      </c>
+      <c r="X9" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y9" s="15"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="U1" s="4" t="s">
+      <c r="B10" s="13" t="str">
+        <f>STANDARD_DEFINITION!B10</f>
+        <v>Concrete and Masonry from 2010's to 2020's</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M10" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="N10" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="O10" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="P10" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>0</v>
+      </c>
+      <c r="R10" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="S10" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="T10" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="U10" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="V10" s="6">
+        <v>0</v>
+      </c>
+      <c r="W10" s="6">
+        <v>0</v>
+      </c>
+      <c r="X10" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y10" s="15"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="13" t="str">
+        <f>STANDARD_DEFINITION!B11</f>
+        <v>Concrete and Masonry (Minergie A)</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="N11" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="O11" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="P11" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>0</v>
+      </c>
+      <c r="R11" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="S11" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="T11" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="U11" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="V11" s="6">
+        <v>0</v>
+      </c>
+      <c r="W11" s="6">
+        <v>0</v>
+      </c>
+      <c r="X11" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y11" s="15"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="V1" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="B12" s="13" t="str">
+        <f>STANDARD_DEFINITION!B12</f>
+        <v>Stone and Masonry before 1900's (renovated)</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I12" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="J12" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="N12" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="O12" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="P12" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="6">
+        <v>0</v>
+      </c>
+      <c r="R12" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="S12" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="T12" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="U12" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="V12" s="6">
+        <v>0</v>
+      </c>
+      <c r="W12" s="6">
+        <v>0</v>
+      </c>
+      <c r="X12" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y12" s="15"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="13" t="str">
+        <f>STANDARD_DEFINITION!B13</f>
+        <v>Concrete and Masonry from 1900's to 1930's  (renovated)</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="J13" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="N13" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="P13" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="6">
+        <v>0</v>
+      </c>
+      <c r="R13" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="S13" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="T13" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="U13" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="V13" s="6">
+        <v>0</v>
+      </c>
+      <c r="W13" s="6">
+        <v>0</v>
+      </c>
+      <c r="X13" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y13" s="15"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" s="13" t="str">
+        <f>STANDARD_DEFINITION!B14</f>
+        <v>Concrete and Masonry from 1930s to 1960's  (renovated)</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="J14" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="N14" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="O14" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="P14" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="6">
+        <v>0</v>
+      </c>
+      <c r="R14" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="S14" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="T14" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="U14" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="V14" s="6">
+        <v>0</v>
+      </c>
+      <c r="W14" s="6">
+        <v>0</v>
+      </c>
+      <c r="X14" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y14" s="15"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B15" s="13" t="str">
+        <f>STANDARD_DEFINITION!B15</f>
+        <v>Concrete and Masonry from 1960's to 1970's  (renovated)</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="L2" s="2">
-        <v>0.82</v>
-      </c>
-      <c r="M2" s="2">
-        <v>0.82</v>
-      </c>
-      <c r="N2" s="2">
-        <v>0.82</v>
-      </c>
-      <c r="O2" s="7">
-        <v>0</v>
-      </c>
-      <c r="P2" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>0.16</v>
-      </c>
-      <c r="R2" s="2">
-        <v>0.16</v>
-      </c>
-      <c r="S2" s="2">
-        <v>0.16</v>
-      </c>
-      <c r="T2" s="2">
-        <v>0.16</v>
-      </c>
-      <c r="U2" s="6">
-        <v>0</v>
-      </c>
-      <c r="V2" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="D15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="J15" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="N15" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="O15" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="P15" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="6">
+        <v>0</v>
+      </c>
+      <c r="R15" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="S15" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="T15" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="U15" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="V15" s="6">
+        <v>0</v>
+      </c>
+      <c r="W15" s="6">
+        <v>0</v>
+      </c>
+      <c r="X15" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y15" s="15"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16" s="13" t="str">
+        <f>STANDARD_DEFINITION!B16</f>
+        <v>Concrete and Masonry from 1970's to 1980's  (renovated)</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="L3" s="2">
-        <v>0.82</v>
-      </c>
-      <c r="M3" s="2">
-        <v>0.82</v>
-      </c>
-      <c r="N3" s="2">
-        <v>0.82</v>
-      </c>
-      <c r="O3" s="7">
-        <v>0</v>
-      </c>
-      <c r="P3" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>0.21</v>
-      </c>
-      <c r="R3" s="2">
-        <v>0.21</v>
-      </c>
-      <c r="S3" s="2">
-        <v>0.21</v>
-      </c>
-      <c r="T3" s="2">
-        <v>0.21</v>
-      </c>
-      <c r="U3" s="6">
-        <v>0</v>
-      </c>
-      <c r="V3" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="D16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="J16" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="N16" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="O16" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="P16" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="6">
+        <v>0</v>
+      </c>
+      <c r="R16" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="S16" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="T16" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="U16" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="V16" s="6">
+        <v>0</v>
+      </c>
+      <c r="W16" s="6">
+        <v>0</v>
+      </c>
+      <c r="X16" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y16" s="15"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" s="13" t="str">
+        <f>STANDARD_DEFINITION!B17</f>
+        <v>Concrete and Masonry from 1980's to 1990's  (renovated)</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="L4" s="2">
-        <v>0.82</v>
-      </c>
-      <c r="M4" s="2">
-        <v>0.82</v>
-      </c>
-      <c r="N4" s="2">
-        <v>0.82</v>
-      </c>
-      <c r="O4" s="7">
-        <v>0</v>
-      </c>
-      <c r="P4" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="R4" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="S4" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="T4" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="U4" s="6">
-        <v>0</v>
-      </c>
-      <c r="V4" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="D17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="J17" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="K17" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M17" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="N17" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="O17" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="P17" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="6">
+        <v>0</v>
+      </c>
+      <c r="R17" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="S17" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="T17" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="U17" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="V17" s="6">
+        <v>0</v>
+      </c>
+      <c r="W17" s="6">
+        <v>0</v>
+      </c>
+      <c r="X17" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y17" s="15"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B18" s="13" t="str">
+        <f>STANDARD_DEFINITION!B18</f>
+        <v>Concrete and Masonry from 1990's to 2000's  (renovated)</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="L5" s="2">
-        <v>0.82</v>
-      </c>
-      <c r="M5" s="2">
-        <v>0.82</v>
-      </c>
-      <c r="N5" s="2">
-        <v>0.82</v>
-      </c>
-      <c r="O5" s="7">
-        <v>0</v>
-      </c>
-      <c r="P5" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>0.21</v>
-      </c>
-      <c r="R5" s="2">
-        <v>0.21</v>
-      </c>
-      <c r="S5" s="2">
-        <v>0.21</v>
-      </c>
-      <c r="T5" s="2">
-        <v>0.21</v>
-      </c>
-      <c r="U5" s="6">
-        <v>0</v>
-      </c>
-      <c r="V5" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="E18" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="J18" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="L6" s="2">
-        <v>0.82</v>
-      </c>
-      <c r="M6" s="2">
-        <v>0.82</v>
-      </c>
-      <c r="N6" s="2">
-        <v>0.82</v>
-      </c>
-      <c r="O6" s="7">
-        <v>0</v>
-      </c>
-      <c r="P6" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="R6" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="S6" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="T6" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="U6" s="6">
-        <v>0</v>
-      </c>
-      <c r="V6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="K18" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="L7" s="2">
-        <v>0.82</v>
-      </c>
-      <c r="M7" s="2">
-        <v>0.82</v>
-      </c>
-      <c r="N7" s="2">
-        <v>0.82</v>
-      </c>
-      <c r="O7" s="7">
-        <v>0</v>
-      </c>
-      <c r="P7" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="R7" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="S7" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="T7" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="U7" s="6">
-        <v>0</v>
-      </c>
-      <c r="V7" s="6">
-        <v>0</v>
-      </c>
+      <c r="L18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M18" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="N18" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="O18" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="P18" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="6">
+        <v>0</v>
+      </c>
+      <c r="R18" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="S18" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="T18" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="U18" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="V18" s="6">
+        <v>0</v>
+      </c>
+      <c r="W18" s="6">
+        <v>0</v>
+      </c>
+      <c r="X18" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y18" s="15"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="X2" r:id="rId1" display="https://enbau-online.ch/bautechnik-der-gebaeudehuelle/1-3%e2%80%82gebaeudehuelle-seit-1900/" xr:uid="{42C11F4B-2409-4225-9304-03185A29E2EA}"/>
+    <hyperlink ref="X3:X18" r:id="rId2" display="https://enbau-online.ch/bautechnik-der-gebaeudehuelle/1-3%e2%80%82gebaeudehuelle-seit-1900/" xr:uid="{5C7D3EC3-7290-4B40-9472-F502E9170840}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>50</v>
+      <c r="B2" s="13" t="str">
+        <f>STANDARD_DEFINITION!B2</f>
+        <v>Stone and Masonry before 1900's</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>50</v>
+      <c r="B3" s="13" t="str">
+        <f>STANDARD_DEFINITION!B3</f>
+        <v>Concrete and Masonry from 1900's to 1930's</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>50</v>
+      <c r="B4" s="13" t="str">
+        <f>STANDARD_DEFINITION!B4</f>
+        <v>Concrete and Masonry from 1930s to 1960's</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>50</v>
+      <c r="B5" s="13" t="str">
+        <f>STANDARD_DEFINITION!B5</f>
+        <v>Concrete and Masonry from 1960's to 1970's</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>51</v>
+      <c r="B6" s="13" t="str">
+        <f>STANDARD_DEFINITION!B6</f>
+        <v>Concrete and Masonry from 1970's to 1980's</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>51</v>
+      <c r="B7" s="13" t="str">
+        <f>STANDARD_DEFINITION!B7</f>
+        <v>Concrete and Masonry from 1980's to 1990's</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>55</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>22</v>
       </c>
     </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="13" t="str">
+        <f>STANDARD_DEFINITION!B8</f>
+        <v>Concrete and Masonry from 1990's to 2000's</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" s="13" t="str">
+        <f>STANDARD_DEFINITION!B9</f>
+        <v>Concrete and Masonry from 2000's to 2010's</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="13" t="str">
+        <f>STANDARD_DEFINITION!B10</f>
+        <v>Concrete and Masonry from 2010's to 2020's</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" s="13" t="str">
+        <f>STANDARD_DEFINITION!B11</f>
+        <v>Concrete and Masonry (Minergie A)</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" s="13" t="str">
+        <f>STANDARD_DEFINITION!B12</f>
+        <v>Stone and Masonry before 1900's (renovated)</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B13" s="13" t="str">
+        <f>STANDARD_DEFINITION!B13</f>
+        <v>Concrete and Masonry from 1900's to 1930's  (renovated)</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B14" s="13" t="str">
+        <f>STANDARD_DEFINITION!B14</f>
+        <v>Concrete and Masonry from 1930s to 1960's  (renovated)</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" s="13" t="str">
+        <f>STANDARD_DEFINITION!B15</f>
+        <v>Concrete and Masonry from 1960's to 1970's  (renovated)</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B16" s="13" t="str">
+        <f>STANDARD_DEFINITION!B16</f>
+        <v>Concrete and Masonry from 1970's to 1980's  (renovated)</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B17" s="13" t="str">
+        <f>STANDARD_DEFINITION!B17</f>
+        <v>Concrete and Masonry from 1980's to 1990's  (renovated)</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B18" s="13" t="str">
+        <f>STANDARD_DEFINITION!B18</f>
+        <v>Concrete and Masonry from 1990's to 2000's  (renovated)</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2074,162 +3754,407 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="13.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="50" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>56</v>
+      <c r="B2" s="13" t="str">
+        <f>STANDARD_DEFINITION!B2</f>
+        <v>Stone and Masonry before 1900's</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>56</v>
+      <c r="B3" s="13" t="str">
+        <f>STANDARD_DEFINITION!B3</f>
+        <v>Concrete and Masonry from 1900's to 1930's</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>56</v>
+      <c r="B4" s="13" t="str">
+        <f>STANDARD_DEFINITION!B4</f>
+        <v>Concrete and Masonry from 1930s to 1960's</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>56</v>
+      <c r="B5" s="13" t="str">
+        <f>STANDARD_DEFINITION!B5</f>
+        <v>Concrete and Masonry from 1960's to 1970's</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>57</v>
+      <c r="B6" s="13" t="str">
+        <f>STANDARD_DEFINITION!B6</f>
+        <v>Concrete and Masonry from 1970's to 1980's</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>57</v>
+      <c r="B7" s="13" t="str">
+        <f>STANDARD_DEFINITION!B7</f>
+        <v>Concrete and Masonry from 1980's to 1990's</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>61</v>
+        <v>53</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="13" t="str">
+        <f>STANDARD_DEFINITION!B8</f>
+        <v>Concrete and Masonry from 1990's to 2000's</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" s="13" t="str">
+        <f>STANDARD_DEFINITION!B9</f>
+        <v>Concrete and Masonry from 2000's to 2010's</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="13" t="str">
+        <f>STANDARD_DEFINITION!B10</f>
+        <v>Concrete and Masonry from 2010's to 2020's</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" s="13" t="str">
+        <f>STANDARD_DEFINITION!B11</f>
+        <v>Concrete and Masonry (Minergie A)</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" s="13" t="str">
+        <f>STANDARD_DEFINITION!B12</f>
+        <v>Stone and Masonry before 1900's (renovated)</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B13" s="13" t="str">
+        <f>STANDARD_DEFINITION!B13</f>
+        <v>Concrete and Masonry from 1900's to 1930's  (renovated)</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B14" s="13" t="str">
+        <f>STANDARD_DEFINITION!B14</f>
+        <v>Concrete and Masonry from 1930s to 1960's  (renovated)</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" s="13" t="str">
+        <f>STANDARD_DEFINITION!B15</f>
+        <v>Concrete and Masonry from 1960's to 1970's  (renovated)</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B16" s="13" t="str">
+        <f>STANDARD_DEFINITION!B16</f>
+        <v>Concrete and Masonry from 1970's to 1980's  (renovated)</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B17" s="13" t="str">
+        <f>STANDARD_DEFINITION!B17</f>
+        <v>Concrete and Masonry from 1980's to 1990's  (renovated)</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B18" s="13" t="str">
+        <f>STANDARD_DEFINITION!B18</f>
+        <v>Concrete and Masonry from 1990's to 2000's  (renovated)</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C4119BA2A2C9A34A9ABDCD539C093B2A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2036187cb88b360b5a6de576d0a5f2f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="be70d004-d1e5-4317-a402-eff109a4a2bb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e63961df46f11abd186e13992df6f3c7" ns3:_="">
     <xsd:import namespace="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
@@ -2399,31 +4324,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02AC8DD-FE6B-486F-A4E4-4D415B112715}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2439,4 +4355,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updating database to reduce arguments
</commit_message>
<xml_diff>
--- a/cea/databases/CH/archetypes/CONSTRUCTION_STANDARD.xlsx
+++ b/cea/databases/CH/archetypes/CONSTRUCTION_STANDARD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ebpgroup-my.sharepoint.com/personal/jimeno_fonseca_ebp_ch/Documents/Dokumente/CityEnergyAnalyst/CityEnergyAnalyst/cea/databases/CH/archetypes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fonseca/Documents/GitHub/CityEnergyAnalyst/cea/databases/CH/archetypes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="503" documentId="11_FC738FCD21D91416D512F37F2E5BB974BC1D8DF6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54195132-CBA8-4347-9190-831E8686D5E4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648B9418-0FA5-5648-BAA2-39592E4375C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45090" yWindow="2400" windowWidth="24810" windowHeight="15600" tabRatio="785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38340" yWindow="-8600" windowWidth="34700" windowHeight="15600" tabRatio="785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STANDARD_DEFINITION" sheetId="10" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="130">
   <si>
     <t>type_hs</t>
   </si>
@@ -285,9 +285,6 @@
     <t>area_balcon</t>
   </si>
   <si>
-    <t>area_pv</t>
-  </si>
-  <si>
     <t>STANDARD7</t>
   </si>
   <si>
@@ -384,9 +381,6 @@
     <t>Concrete and Masonry from 1990's to 2000's  (renovated)</t>
   </si>
   <si>
-    <t>Refernez</t>
-  </si>
-  <si>
     <t>1.3 Gebäudehülle seit 1900 | Bautechnik der Gebäudehülle (enbau-online.ch)</t>
   </si>
   <si>
@@ -429,13 +423,13 @@
     <t>STANDARD17</t>
   </si>
   <si>
-    <t>area_sc</t>
-  </si>
-  <si>
     <t>type_col</t>
   </si>
   <si>
     <t>COLUMN_AS0</t>
+  </si>
+  <si>
+    <t>Reference</t>
   </si>
 </sst>
 </file>
@@ -602,7 +596,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="35">
@@ -974,7 +968,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -995,16 +989,13 @@
     <xf numFmtId="164" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1344,19 +1335,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="59.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="59.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
@@ -1370,12 +1361,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>40</v>
@@ -1384,49 +1375,49 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D3" s="10">
         <v>1930</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D4" s="10">
         <v>1960</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D5" s="10">
         <v>1970</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -1440,82 +1431,82 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="10">
         <v>1990</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" s="10">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C8" s="8" t="s">
+      <c r="B9" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="D8" s="11">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="C9" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="10">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B10" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C10" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="D9" s="11">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="D10" s="10">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="D10" s="11">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="B11" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D11" s="11">
+        <v>98</v>
+      </c>
+      <c r="D11" s="10">
         <v>2015</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>40</v>
@@ -1524,54 +1515,54 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D13" s="10">
         <v>1930</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D14" s="10">
         <v>1960</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D15" s="10">
         <v>1970</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>41</v>
@@ -1580,31 +1571,31 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="10">
         <v>1990</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="D18" s="11">
+        <v>100</v>
+      </c>
+      <c r="D18" s="10">
         <v>2000</v>
       </c>
     </row>
@@ -1619,44 +1610,41 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AA18"/>
+  <dimension ref="A1:Y18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L2" sqref="L2:L18"/>
+      <selection pane="bottomRight" activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="50" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" style="1" customWidth="1"/>
     <col min="7" max="8" width="11" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13.5" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.28515625" style="1" customWidth="1"/>
-    <col min="25" max="25" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="1"/>
+    <col min="19" max="19" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
@@ -1691,7 +1679,7 @@
         <v>75</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>4</v>
@@ -1724,24 +1712,18 @@
         <v>14</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="X1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X1" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="Y1" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="Z1" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="AA1" s="15"/>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Y1" s="14"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="13" t="str">
+      <c r="B2" s="12" t="str">
         <f>STANDARD_DEFINITION!B2</f>
         <v>Stone and Masonry before 1900's</v>
       </c>
@@ -1749,31 +1731,31 @@
         <v>71</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>61</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="K2" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H2" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="L2" s="18" t="s">
-        <v>131</v>
+      <c r="L2" s="17" t="s">
+        <v>128</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>64</v>
@@ -1808,22 +1790,16 @@
       <c r="W2" s="6">
         <v>0</v>
       </c>
-      <c r="X2" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="AA2" s="15"/>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="X2" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y2" s="14"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="13" t="str">
+      <c r="B3" s="12" t="str">
         <f>STANDARD_DEFINITION!B3</f>
         <v>Concrete and Masonry from 1900's to 1930's</v>
       </c>
@@ -1831,31 +1807,31 @@
         <v>71</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>61</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="K3" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H3" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="J3" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="L3" s="18" t="s">
-        <v>131</v>
+      <c r="L3" s="17" t="s">
+        <v>128</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>64</v>
@@ -1890,22 +1866,16 @@
       <c r="W3" s="6">
         <v>0</v>
       </c>
-      <c r="X3" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="AA3" s="15"/>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="X3" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y3" s="14"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="13" t="str">
+      <c r="B4" s="12" t="str">
         <f>STANDARD_DEFINITION!B4</f>
         <v>Concrete and Masonry from 1930s to 1960's</v>
       </c>
@@ -1913,31 +1883,31 @@
         <v>71</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="13" t="s">
         <v>60</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="J4" s="17" t="s">
+      <c r="J4" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="K4" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="L4" s="18" t="s">
-        <v>131</v>
+      <c r="K4" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>128</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>64</v>
@@ -1972,22 +1942,16 @@
       <c r="W4" s="6">
         <v>0</v>
       </c>
-      <c r="X4" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="AA4" s="15"/>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="X4" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y4" s="14"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="13" t="str">
+      <c r="B5" s="12" t="str">
         <f>STANDARD_DEFINITION!B5</f>
         <v>Concrete and Masonry from 1960's to 1970's</v>
       </c>
@@ -2000,26 +1964,26 @@
       <c r="E5" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="13" t="s">
         <v>60</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="K5" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="J5" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="K5" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="L5" s="18" t="s">
-        <v>131</v>
+      <c r="L5" s="17" t="s">
+        <v>128</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>64</v>
@@ -2054,22 +2018,16 @@
       <c r="W5" s="6">
         <v>0</v>
       </c>
-      <c r="X5" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="AA5" s="15"/>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="X5" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y5" s="14"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="13" t="str">
+      <c r="B6" s="12" t="str">
         <f>STANDARD_DEFINITION!B6</f>
         <v>Concrete and Masonry from 1970's to 1980's</v>
       </c>
@@ -2082,26 +2040,26 @@
       <c r="E6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="13" t="s">
         <v>60</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="K6" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="K6" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="L6" s="18" t="s">
-        <v>131</v>
+      <c r="L6" s="17" t="s">
+        <v>128</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>63</v>
@@ -2136,22 +2094,16 @@
       <c r="W6" s="6">
         <v>0</v>
       </c>
-      <c r="X6" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="AA6" s="15"/>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="X6" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y6" s="14"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="13" t="str">
+      <c r="B7" s="12" t="str">
         <f>STANDARD_DEFINITION!B7</f>
         <v>Concrete and Masonry from 1980's to 1990's</v>
       </c>
@@ -2162,28 +2114,28 @@
         <v>68</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F7" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" s="13" t="s">
         <v>60</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="J7" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="J7" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="L7" s="18" t="s">
-        <v>131</v>
+      <c r="L7" s="17" t="s">
+        <v>128</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>63</v>
@@ -2218,22 +2170,16 @@
       <c r="W7" s="6">
         <v>0</v>
       </c>
-      <c r="X7" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="AA7" s="15"/>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="X7" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y7" s="14"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B8" s="13" t="str">
+        <v>81</v>
+      </c>
+      <c r="B8" s="12" t="str">
         <f>STANDARD_DEFINITION!B8</f>
         <v>Concrete and Masonry from 1990's to 2000's</v>
       </c>
@@ -2244,28 +2190,28 @@
         <v>68</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F8" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8" s="13" t="s">
         <v>60</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="J8" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="J8" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="K8" s="12" t="s">
+      <c r="K8" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="L8" s="18" t="s">
-        <v>131</v>
+      <c r="L8" s="17" t="s">
+        <v>128</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>63</v>
@@ -2300,22 +2246,16 @@
       <c r="W8" s="6">
         <v>0</v>
       </c>
-      <c r="X8" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="AA8" s="15"/>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="X8" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y8" s="14"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" s="13" t="str">
+        <v>82</v>
+      </c>
+      <c r="B9" s="12" t="str">
         <f>STANDARD_DEFINITION!B9</f>
         <v>Concrete and Masonry from 2000's to 2010's</v>
       </c>
@@ -2326,28 +2266,28 @@
         <v>69</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H9" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="J9" s="17" t="s">
+      <c r="J9" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="L9" s="18" t="s">
-        <v>131</v>
+      <c r="L9" s="17" t="s">
+        <v>128</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>63</v>
@@ -2382,22 +2322,16 @@
       <c r="W9" s="6">
         <v>0</v>
       </c>
-      <c r="X9" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="AA9" s="15"/>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="X9" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y9" s="14"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" s="13" t="str">
+        <v>83</v>
+      </c>
+      <c r="B10" s="12" t="str">
         <f>STANDARD_DEFINITION!B10</f>
         <v>Concrete and Masonry from 2010's to 2020's</v>
       </c>
@@ -2411,25 +2345,25 @@
         <v>67</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H10" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="J10" s="17" t="s">
+      <c r="J10" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="K10" s="12" t="s">
+      <c r="K10" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="L10" s="18" t="s">
-        <v>131</v>
+      <c r="L10" s="17" t="s">
+        <v>128</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>63</v>
@@ -2464,22 +2398,16 @@
       <c r="W10" s="6">
         <v>0</v>
       </c>
-      <c r="X10" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="AA10" s="15"/>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="X10" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y10" s="14"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" s="13" t="str">
+        <v>84</v>
+      </c>
+      <c r="B11" s="12" t="str">
         <f>STANDARD_DEFINITION!B11</f>
         <v>Concrete and Masonry (Minergie A)</v>
       </c>
@@ -2496,22 +2424,22 @@
         <v>62</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H11" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="J11" s="17" t="s">
+      <c r="J11" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="K11" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="L11" s="18" t="s">
-        <v>131</v>
+      <c r="L11" s="17" t="s">
+        <v>128</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>63</v>
@@ -2546,22 +2474,16 @@
       <c r="W11" s="6">
         <v>0</v>
       </c>
-      <c r="X11" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="AA11" s="15"/>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="X11" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y11" s="14"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B12" s="13" t="str">
+        <v>120</v>
+      </c>
+      <c r="B12" s="12" t="str">
         <f>STANDARD_DEFINITION!B12</f>
         <v>Stone and Masonry before 1900's (renovated)</v>
       </c>
@@ -2572,28 +2494,28 @@
         <v>68</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>106</v>
+        <v>88</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>105</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="I12" s="12" t="s">
+      <c r="I12" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="J12" s="17" t="s">
+      <c r="J12" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="K12" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="L12" s="18" t="s">
-        <v>131</v>
+      <c r="K12" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="L12" s="17" t="s">
+        <v>128</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>64</v>
@@ -2628,22 +2550,16 @@
       <c r="W12" s="6">
         <v>0</v>
       </c>
-      <c r="X12" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="AA12" s="15"/>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="X12" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y12" s="14"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B13" s="13" t="str">
+        <v>121</v>
+      </c>
+      <c r="B13" s="12" t="str">
         <f>STANDARD_DEFINITION!B13</f>
         <v>Concrete and Masonry from 1900's to 1930's  (renovated)</v>
       </c>
@@ -2654,28 +2570,28 @@
         <v>68</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>106</v>
+        <v>88</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>105</v>
       </c>
       <c r="G13" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="J13" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="K13" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="J13" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="K13" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="L13" s="18" t="s">
-        <v>131</v>
+      <c r="L13" s="17" t="s">
+        <v>128</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>64</v>
@@ -2710,22 +2626,16 @@
       <c r="W13" s="6">
         <v>0</v>
       </c>
-      <c r="X13" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="AA13" s="15"/>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="X13" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y13" s="14"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B14" s="13" t="str">
+        <v>122</v>
+      </c>
+      <c r="B14" s="12" t="str">
         <f>STANDARD_DEFINITION!B14</f>
         <v>Concrete and Masonry from 1930s to 1960's  (renovated)</v>
       </c>
@@ -2736,28 +2646,28 @@
         <v>68</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>106</v>
+        <v>88</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>105</v>
       </c>
       <c r="G14" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="K14" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="J14" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="L14" s="18" t="s">
-        <v>131</v>
+      <c r="L14" s="17" t="s">
+        <v>128</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>64</v>
@@ -2792,22 +2702,16 @@
       <c r="W14" s="6">
         <v>0</v>
       </c>
-      <c r="X14" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="AA14" s="15"/>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="X14" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y14" s="14"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B15" s="13" t="str">
+        <v>123</v>
+      </c>
+      <c r="B15" s="12" t="str">
         <f>STANDARD_DEFINITION!B15</f>
         <v>Concrete and Masonry from 1960's to 1970's  (renovated)</v>
       </c>
@@ -2818,28 +2722,28 @@
         <v>68</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>106</v>
+        <v>88</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>105</v>
       </c>
       <c r="G15" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="J15" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="K15" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="I15" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="J15" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="K15" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="L15" s="18" t="s">
-        <v>131</v>
+      <c r="L15" s="17" t="s">
+        <v>128</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>64</v>
@@ -2874,22 +2778,16 @@
       <c r="W15" s="6">
         <v>0</v>
       </c>
-      <c r="X15" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z15" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="AA15" s="15"/>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="X15" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y15" s="14"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B16" s="13" t="str">
+        <v>124</v>
+      </c>
+      <c r="B16" s="12" t="str">
         <f>STANDARD_DEFINITION!B16</f>
         <v>Concrete and Masonry from 1970's to 1980's  (renovated)</v>
       </c>
@@ -2900,28 +2798,28 @@
         <v>68</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G16" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="J16" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="K16" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="I16" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="J16" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="K16" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="L16" s="18" t="s">
-        <v>131</v>
+      <c r="L16" s="17" t="s">
+        <v>128</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>63</v>
@@ -2956,22 +2854,16 @@
       <c r="W16" s="6">
         <v>0</v>
       </c>
-      <c r="X16" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z16" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="AA16" s="15"/>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="X16" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y16" s="14"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B17" s="13" t="str">
+        <v>125</v>
+      </c>
+      <c r="B17" s="12" t="str">
         <f>STANDARD_DEFINITION!B17</f>
         <v>Concrete and Masonry from 1980's to 1990's  (renovated)</v>
       </c>
@@ -2982,28 +2874,28 @@
         <v>68</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H17" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="I17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="J17" s="17" t="s">
+      <c r="J17" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="K17" s="12" t="s">
+      <c r="K17" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="L17" s="18" t="s">
-        <v>131</v>
+      <c r="L17" s="17" t="s">
+        <v>128</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>63</v>
@@ -3038,22 +2930,16 @@
       <c r="W17" s="6">
         <v>0</v>
       </c>
-      <c r="X17" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y17" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="AA17" s="15"/>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="X17" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y17" s="14"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B18" s="13" t="str">
+        <v>126</v>
+      </c>
+      <c r="B18" s="12" t="str">
         <f>STANDARD_DEFINITION!B18</f>
         <v>Concrete and Masonry from 1990's to 2000's  (renovated)</v>
       </c>
@@ -3064,28 +2950,28 @@
         <v>68</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H18" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="I18" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="J18" s="17" t="s">
+      <c r="J18" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="K18" s="12" t="s">
+      <c r="K18" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="L18" s="18" t="s">
-        <v>131</v>
+      <c r="L18" s="17" t="s">
+        <v>128</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>63</v>
@@ -3120,22 +3006,16 @@
       <c r="W18" s="6">
         <v>0</v>
       </c>
-      <c r="X18" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y18" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="AA18" s="15"/>
+      <c r="X18" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y18" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="Z2" r:id="rId1" display="https://enbau-online.ch/bautechnik-der-gebaeudehuelle/1-3%e2%80%82gebaeudehuelle-seit-1900/" xr:uid="{42C11F4B-2409-4225-9304-03185A29E2EA}"/>
-    <hyperlink ref="Z3:Z18" r:id="rId2" display="https://enbau-online.ch/bautechnik-der-gebaeudehuelle/1-3%e2%80%82gebaeudehuelle-seit-1900/" xr:uid="{5C7D3EC3-7290-4B40-9472-F502E9170840}"/>
+    <hyperlink ref="X2" r:id="rId1" display="https://enbau-online.ch/bautechnik-der-gebaeudehuelle/1-3%e2%80%82gebaeudehuelle-seit-1900/" xr:uid="{42C11F4B-2409-4225-9304-03185A29E2EA}"/>
+    <hyperlink ref="X3:X18" r:id="rId2" display="https://enbau-online.ch/bautechnik-der-gebaeudehuelle/1-3%e2%80%82gebaeudehuelle-seit-1900/" xr:uid="{5C7D3EC3-7290-4B40-9472-F502E9170840}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -3153,21 +3033,21 @@
       <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5" style="3" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
@@ -3202,11 +3082,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="13" t="str">
+      <c r="B2" s="12" t="str">
         <f>STANDARD_DEFINITION!B2</f>
         <v>Stone and Masonry before 1900's</v>
       </c>
@@ -3238,11 +3118,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="13" t="str">
+      <c r="B3" s="12" t="str">
         <f>STANDARD_DEFINITION!B3</f>
         <v>Concrete and Masonry from 1900's to 1930's</v>
       </c>
@@ -3274,11 +3154,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="13" t="str">
+      <c r="B4" s="12" t="str">
         <f>STANDARD_DEFINITION!B4</f>
         <v>Concrete and Masonry from 1930s to 1960's</v>
       </c>
@@ -3310,11 +3190,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="13" t="str">
+      <c r="B5" s="12" t="str">
         <f>STANDARD_DEFINITION!B5</f>
         <v>Concrete and Masonry from 1960's to 1970's</v>
       </c>
@@ -3346,11 +3226,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="13" t="str">
+      <c r="B6" s="12" t="str">
         <f>STANDARD_DEFINITION!B6</f>
         <v>Concrete and Masonry from 1970's to 1980's</v>
       </c>
@@ -3382,11 +3262,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="13" t="str">
+      <c r="B7" s="12" t="str">
         <f>STANDARD_DEFINITION!B7</f>
         <v>Concrete and Masonry from 1980's to 1990's</v>
       </c>
@@ -3418,11 +3298,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B8" s="13" t="str">
+        <v>81</v>
+      </c>
+      <c r="B8" s="12" t="str">
         <f>STANDARD_DEFINITION!B8</f>
         <v>Concrete and Masonry from 1990's to 2000's</v>
       </c>
@@ -3454,11 +3334,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" s="13" t="str">
+        <v>82</v>
+      </c>
+      <c r="B9" s="12" t="str">
         <f>STANDARD_DEFINITION!B9</f>
         <v>Concrete and Masonry from 2000's to 2010's</v>
       </c>
@@ -3490,11 +3370,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" s="13" t="str">
+        <v>83</v>
+      </c>
+      <c r="B10" s="12" t="str">
         <f>STANDARD_DEFINITION!B10</f>
         <v>Concrete and Masonry from 2010's to 2020's</v>
       </c>
@@ -3526,11 +3406,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" s="13" t="str">
+        <v>84</v>
+      </c>
+      <c r="B11" s="12" t="str">
         <f>STANDARD_DEFINITION!B11</f>
         <v>Concrete and Masonry (Minergie A)</v>
       </c>
@@ -3562,11 +3442,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B12" s="13" t="str">
+        <v>120</v>
+      </c>
+      <c r="B12" s="12" t="str">
         <f>STANDARD_DEFINITION!B12</f>
         <v>Stone and Masonry before 1900's (renovated)</v>
       </c>
@@ -3598,11 +3478,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B13" s="13" t="str">
+        <v>121</v>
+      </c>
+      <c r="B13" s="12" t="str">
         <f>STANDARD_DEFINITION!B13</f>
         <v>Concrete and Masonry from 1900's to 1930's  (renovated)</v>
       </c>
@@ -3634,11 +3514,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B14" s="13" t="str">
+        <v>122</v>
+      </c>
+      <c r="B14" s="12" t="str">
         <f>STANDARD_DEFINITION!B14</f>
         <v>Concrete and Masonry from 1930s to 1960's  (renovated)</v>
       </c>
@@ -3670,11 +3550,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B15" s="13" t="str">
+        <v>123</v>
+      </c>
+      <c r="B15" s="12" t="str">
         <f>STANDARD_DEFINITION!B15</f>
         <v>Concrete and Masonry from 1960's to 1970's  (renovated)</v>
       </c>
@@ -3706,11 +3586,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B16" s="13" t="str">
+        <v>124</v>
+      </c>
+      <c r="B16" s="12" t="str">
         <f>STANDARD_DEFINITION!B16</f>
         <v>Concrete and Masonry from 1970's to 1980's  (renovated)</v>
       </c>
@@ -3742,11 +3622,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B17" s="13" t="str">
+        <v>125</v>
+      </c>
+      <c r="B17" s="12" t="str">
         <f>STANDARD_DEFINITION!B17</f>
         <v>Concrete and Masonry from 1980's to 1990's  (renovated)</v>
       </c>
@@ -3778,11 +3658,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B18" s="13" t="str">
+        <v>126</v>
+      </c>
+      <c r="B18" s="12" t="str">
         <f>STANDARD_DEFINITION!B18</f>
         <v>Concrete and Masonry from 1990's to 2000's  (renovated)</v>
       </c>
@@ -3826,21 +3706,21 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" style="5" customWidth="1"/>
     <col min="2" max="2" width="50" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="20.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
@@ -3860,11 +3740,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="13" t="str">
+      <c r="B2" s="12" t="str">
         <f>STANDARD_DEFINITION!B2</f>
         <v>Stone and Masonry before 1900's</v>
       </c>
@@ -3881,11 +3761,11 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="13" t="str">
+      <c r="B3" s="12" t="str">
         <f>STANDARD_DEFINITION!B3</f>
         <v>Concrete and Masonry from 1900's to 1930's</v>
       </c>
@@ -3902,11 +3782,11 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="13" t="str">
+      <c r="B4" s="12" t="str">
         <f>STANDARD_DEFINITION!B4</f>
         <v>Concrete and Masonry from 1930s to 1960's</v>
       </c>
@@ -3923,11 +3803,11 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="13" t="str">
+      <c r="B5" s="12" t="str">
         <f>STANDARD_DEFINITION!B5</f>
         <v>Concrete and Masonry from 1960's to 1970's</v>
       </c>
@@ -3944,11 +3824,11 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="13" t="str">
+      <c r="B6" s="12" t="str">
         <f>STANDARD_DEFINITION!B6</f>
         <v>Concrete and Masonry from 1970's to 1980's</v>
       </c>
@@ -3965,11 +3845,11 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="13" t="str">
+      <c r="B7" s="12" t="str">
         <f>STANDARD_DEFINITION!B7</f>
         <v>Concrete and Masonry from 1980's to 1990's</v>
       </c>
@@ -3986,11 +3866,11 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B8" s="13" t="str">
+        <v>81</v>
+      </c>
+      <c r="B8" s="12" t="str">
         <f>STANDARD_DEFINITION!B8</f>
         <v>Concrete and Masonry from 1990's to 2000's</v>
       </c>
@@ -4007,11 +3887,11 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" s="13" t="str">
+        <v>82</v>
+      </c>
+      <c r="B9" s="12" t="str">
         <f>STANDARD_DEFINITION!B9</f>
         <v>Concrete and Masonry from 2000's to 2010's</v>
       </c>
@@ -4028,11 +3908,11 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" s="13" t="str">
+        <v>83</v>
+      </c>
+      <c r="B10" s="12" t="str">
         <f>STANDARD_DEFINITION!B10</f>
         <v>Concrete and Masonry from 2010's to 2020's</v>
       </c>
@@ -4049,11 +3929,11 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" s="13" t="str">
+        <v>84</v>
+      </c>
+      <c r="B11" s="12" t="str">
         <f>STANDARD_DEFINITION!B11</f>
         <v>Concrete and Masonry (Minergie A)</v>
       </c>
@@ -4070,11 +3950,11 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B12" s="13" t="str">
+        <v>120</v>
+      </c>
+      <c r="B12" s="12" t="str">
         <f>STANDARD_DEFINITION!B12</f>
         <v>Stone and Masonry before 1900's (renovated)</v>
       </c>
@@ -4091,11 +3971,11 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B13" s="13" t="str">
+        <v>121</v>
+      </c>
+      <c r="B13" s="12" t="str">
         <f>STANDARD_DEFINITION!B13</f>
         <v>Concrete and Masonry from 1900's to 1930's  (renovated)</v>
       </c>
@@ -4112,11 +3992,11 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B14" s="13" t="str">
+        <v>122</v>
+      </c>
+      <c r="B14" s="12" t="str">
         <f>STANDARD_DEFINITION!B14</f>
         <v>Concrete and Masonry from 1930s to 1960's  (renovated)</v>
       </c>
@@ -4133,11 +4013,11 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B15" s="13" t="str">
+        <v>123</v>
+      </c>
+      <c r="B15" s="12" t="str">
         <f>STANDARD_DEFINITION!B15</f>
         <v>Concrete and Masonry from 1960's to 1970's  (renovated)</v>
       </c>
@@ -4154,11 +4034,11 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B16" s="13" t="str">
+        <v>124</v>
+      </c>
+      <c r="B16" s="12" t="str">
         <f>STANDARD_DEFINITION!B16</f>
         <v>Concrete and Masonry from 1970's to 1980's  (renovated)</v>
       </c>
@@ -4175,11 +4055,11 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B17" s="13" t="str">
+        <v>125</v>
+      </c>
+      <c r="B17" s="12" t="str">
         <f>STANDARD_DEFINITION!B17</f>
         <v>Concrete and Masonry from 1980's to 1990's  (renovated)</v>
       </c>
@@ -4196,11 +4076,11 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B18" s="13" t="str">
+        <v>126</v>
+      </c>
+      <c r="B18" s="12" t="str">
         <f>STANDARD_DEFINITION!B18</f>
         <v>Concrete and Masonry from 1990's to 2000's  (renovated)</v>
       </c>
@@ -4224,12 +4104,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4403,15 +4280,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4435,17 +4323,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
change position of area_pv
</commit_message>
<xml_diff>
--- a/cea/databases/CH/archetypes/CONSTRUCTION_STANDARD.xlsx
+++ b/cea/databases/CH/archetypes/CONSTRUCTION_STANDARD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fonseca/Documents/GitHub/CityEnergyAnalyst/cea/databases/CH/archetypes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648B9418-0FA5-5648-BAA2-39592E4375C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97191C41-3097-A841-95C0-74C80553FE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38340" yWindow="-8600" windowWidth="34700" windowHeight="15600" tabRatio="785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1180" yWindow="5360" windowWidth="30740" windowHeight="11040" tabRatio="785" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STANDARD_DEFINITION" sheetId="10" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="132">
   <si>
     <t>type_hs</t>
   </si>
@@ -430,6 +430,12 @@
   </si>
   <si>
     <t>Reference</t>
+  </si>
+  <si>
+    <t>type_el_pv</t>
+  </si>
+  <si>
+    <t>SUPPLY_ELECTRICITY_PV_AS0</t>
   </si>
 </sst>
 </file>
@@ -1335,7 +1341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A18"/>
     </sheetView>
   </sheetViews>
@@ -3703,10 +3709,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3716,11 +3722,11 @@
     <col min="3" max="3" width="20.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1640625" style="1"/>
+    <col min="6" max="7" width="23.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
@@ -3739,8 +3745,11 @@
       <c r="F1" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -3760,8 +3769,11 @@
       <c r="F2" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
@@ -3781,8 +3793,11 @@
       <c r="F3" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
@@ -3802,8 +3817,11 @@
       <c r="F4" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -3823,8 +3841,11 @@
       <c r="F5" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -3844,8 +3865,11 @@
       <c r="F6" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
@@ -3865,8 +3889,11 @@
       <c r="F7" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>81</v>
       </c>
@@ -3886,8 +3913,11 @@
       <c r="F8" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>82</v>
       </c>
@@ -3907,8 +3937,11 @@
       <c r="F9" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>83</v>
       </c>
@@ -3928,8 +3961,11 @@
       <c r="F10" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>84</v>
       </c>
@@ -3949,8 +3985,11 @@
       <c r="F11" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>120</v>
       </c>
@@ -3970,8 +4009,11 @@
       <c r="F12" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>121</v>
       </c>
@@ -3991,8 +4033,11 @@
       <c r="F13" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>122</v>
       </c>
@@ -4012,8 +4057,11 @@
       <c r="F14" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>123</v>
       </c>
@@ -4033,8 +4081,11 @@
       <c r="F15" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>124</v>
       </c>
@@ -4054,8 +4105,11 @@
       <c r="F16" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>125</v>
       </c>
@@ -4075,8 +4129,11 @@
       <c r="F17" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>126</v>
       </c>
@@ -4095,6 +4152,9 @@
       </c>
       <c r="F18" s="2" t="s">
         <v>54</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update in ENVELOPE dataset
The names of components and standard for the new building's U_Value are updated (to SIA 380) in CH, and the SG datasets are modified.
</commit_message>
<xml_diff>
--- a/cea/databases/CH/archetypes/CONSTRUCTION_STANDARD.xlsx
+++ b/cea/databases/CH/archetypes/CONSTRUCTION_STANDARD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis.santos\Documents\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\CH\archetypes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmeshkin\Documents\GitHub\CityEnergyAnalyst\cea\databases\CH\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30023ACE-ACC8-4E5D-B644-EA5EC2E13074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1904402-D2A8-4C79-8B13-9DB9B230D649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" tabRatio="785" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STANDARD_DEFINITION" sheetId="10" r:id="rId1"/>
@@ -808,7 +808,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -830,16 +830,13 @@
     <xf numFmtId="164" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -901,10 +898,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1173,7 +1166,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1264,7 +1257,7 @@
       <c r="C6" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="11">
         <v>2040</v>
       </c>
     </row>
@@ -1278,7 +1271,7 @@
       <c r="C7" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="11">
         <v>2040</v>
       </c>
     </row>
@@ -1294,7 +1287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1404,10 +1397,10 @@
       <c r="G2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="12" t="s">
         <v>85</v>
       </c>
       <c r="J2" s="2" t="s">
@@ -1464,10 +1457,10 @@
       <c r="G3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="12" t="s">
         <v>87</v>
       </c>
       <c r="J3" s="2" t="s">
@@ -1524,10 +1517,10 @@
       <c r="G4" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="12" t="s">
         <v>87</v>
       </c>
       <c r="J4" s="2" t="s">
@@ -1584,10 +1577,10 @@
       <c r="G5" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="12" t="s">
         <v>87</v>
       </c>
       <c r="J5" s="2" t="s">
@@ -1644,10 +1637,10 @@
       <c r="G6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="12" t="s">
         <v>87</v>
       </c>
       <c r="J6" s="2" t="s">
@@ -1703,10 +1696,10 @@
       <c r="G7" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="12" t="s">
         <v>87</v>
       </c>
       <c r="J7" s="2" t="s">
@@ -2004,7 +1997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -2143,21 +2136,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C4119BA2A2C9A34A9ABDCD539C093B2A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2036187cb88b360b5a6de576d0a5f2f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="be70d004-d1e5-4317-a402-eff109a4a2bb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e63961df46f11abd186e13992df6f3c7" ns3:_="">
     <xsd:import namespace="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
@@ -2327,10 +2305,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02AC8DD-FE6B-486F-A4E4-4D415B112715}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2352,19 +2355,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02AC8DD-FE6B-486F-A4E4-4D415B112715}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>